<commit_message>
Updated form data, fixed authorization on check endpoint
</commit_message>
<xml_diff>
--- a/app-server/src/main/resources/chairs_responses.xlsx
+++ b/app-server/src/main/resources/chairs_responses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/Documents/acm_users/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/code/acmsac/app-server/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D6B4258-381E-A544-93F5-7655FE0BBEFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF85867-C2BC-AF43-99DF-59CFB6A5870B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="3560" windowWidth="26440" windowHeight="15440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chairs_test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="170">
   <si>
     <t>Timestamp</t>
   </si>
@@ -165,11 +165,431 @@
 On behalf of the entire SAC 2020 Organizing Committee, we congratulate all the authors for having their papers accepted in the SE Track. We are grateful to the members of the Program Committee and to the additional reviewers. Without their support, the organization of such high-quality track sessions would not be possible. We also wish to convey our special thanks to the SAC 2020 symposium's main organizers, especially Program Chairs, Dongwan Shin and Alessio Bechini, for their continuous help and advice and Publication Chair, Hossain Shahriar, and Poster Chairs, Alessio Bechini and Miroslav Bures, for their
 invaluable support. </t>
   </si>
+  <si>
+    <t>2020/03/23 1:11:57 AM EST</t>
+  </si>
+  <si>
+    <t>jmjung@hnu.kr</t>
+  </si>
+  <si>
+    <t>Software Platform</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://sites.google.com/site/acmsac20sp/</t>
+  </si>
+  <si>
+    <t>Jinman Jung, Hannam University</t>
+  </si>
+  <si>
+    <t>Juw Won Park, University of Louisville
+Jinman Jung, Hannam University
+Jun Huang, Chongqing University of Post &amp; Telecommunications</t>
+  </si>
+  <si>
+    <t>2020/03/23 3:31:12 AM EST</t>
+  </si>
+  <si>
+    <t>fdivina@upo.es</t>
+  </si>
+  <si>
+    <t>Applications of Evolutionary Computing</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>https://ectracksac2020.wordpress.com/</t>
+  </si>
+  <si>
+    <t>Federico Divina, Pablo de Olavide University</t>
+  </si>
+  <si>
+    <t>Miguel Garc√≠a Torres, Pablo de Olavide University, co-chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We would like to thank all the PC members for their help, and the authors for their collaboration in facing this difficult time. </t>
+  </si>
+  <si>
+    <t>0000-0002-0964-9506</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=SWOsSj8AAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>2020/03/23 3:45:51 AM EST</t>
+  </si>
+  <si>
+    <t>bordogna.g@irea.cnr.it</t>
+  </si>
+  <si>
+    <t>Information Access and Retrieval</t>
+  </si>
+  <si>
+    <t>IAR</t>
+  </si>
+  <si>
+    <t>http://www.irea.cnr.it/en/images/stories/events/CFP_ACM_SAC_IAR_TRACK_2020.pdf</t>
+  </si>
+  <si>
+    <t>Gloria Bordogna (CNR IREA) 
+Gabriella Pasi (univ. Milano Bicocca)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This year IAR track is in its 19th edition in the context of SAC. Its main aim is allowing researchers and practitioners to present and discuss their proposals and experiences in the middle of the theory-practice spectrum of multisource Information Retrieval, Filtering and recommendation.  This year the Track includes three full papers (with an acceptance rate of 25%), and two poster papers. Each paper was peer reviewed by five members of the Program Committee (listed in these proceedings) to whom we express our gratitude: their help has been invaluable for carrying out a high quality selection process. 
+The full papers cover different up to date research topics related to Information Retrieval by distinct machine learning methods: learning to rank, query performance prediction,  IR models for neophytes.
+The first paper entitled  ‚ÄúIterative Learning to Rank from Explicit Relevance Feedback‚Äù by Mateus Malvessi Pereira, Elham Etemad and Fernando Paulovic, considers the implicit or explicit users feedback in order to understand their intent and improve the quality of retrieved documents. They propose a model that combines explicit relevance feedback and learning to rank techniques to improve the quality of retrieved documents. Besides evaluating the proposed method in general information retrieval cases, they applied it to the special case of Community Question Answering (CQA) systems and the evaluation demonstrated that the proposal outperforms other existing learning to rank techniques on most of the datasets of the bechmark.
+The paper entitled ‚ÄúForward and Backward Feature Selection for Query Performance Prediction‚Äù by S√©bastien D√©jean, Radu Tudor Ionescu, Josiane Mothe and Md Zia Ullah, discusses how to automatically estimate the search effectiveness for any given query, without having relevance judgements. State-of-the-art methods employing machine learning are impossible to interpret because of their black-box nature. Nevertheless, an interpretation is useful for understanding the predictive model. With this in mind the authors investigate a new framework for feature selection in which the trained model explains well the prediction. It is founded on a step-wise (forward and backward) model selection approach where different subsets of query features are used to fit different models from which the system selects the best one. They found that the proposal, besides being readable and understandable, is as good as the majority of complex models, and it is better than non-selective models.
+The third paper entitled ‚ÄúEvaluating the Usefulness of Citation Graph and Document Metadata in Scientific Document Recommendation for Neophytes‚Äù by Bissan Audeh, Michel Beigbeder, Christine Largeron and Diana Ram√≠rez faces the problem of improving the retrieval of documents for neophytes engaged in querying digital libraries. Neophytes do not necessarily use appropriate keywords to express their information needs and they are not necessarily qualified to evaluate correctly the relevance of documents. The paper assumes that the retrieval system should take into consideration features other than content-based relevance. To test this hypothesis, they use machine learning methods with content-based index scores and additional features based on the citation graph and document metadata extracted from external resources. The analysis concludes that the use of additional features improves the performance of the system for a neophyte user, since the system is capable of finding more documents suitable for neophytes within the retrieved results than when using content-based features alone.
+The two poster papers are about geographic information retrieval and audio representation learning. 
+The first poster-paper entitled ‚ÄúRetrieval of Visiting Paths through Relevant Resources and Services for Enabling Smart Communities‚Äù by Gloria Bordogna, Luca Frigerio and Anna Rampini, focuses the problem of searching within a multisource collection of both open data, describing authoritative territorial resources, and user generated ADS, describing private services offered in a geographic area. The objective is to enable prioretized and personalized queries capable to generate and rank convenient paths to sequentially visit different resources and services deemed relevant according to the personal user preferences and the geographic context. 
+The second post-paper entitled ‚ÄúUnsupervised Cross-Modal Audio Representation Learning from Unstructured Multilingual Text‚Äù by Alexander Schindler, Sergiu Gordea and Peter Knees is about an approach to unsupervised audio representation learning. Based on a triplet neural network architecture, they harnesses semantically related cross-modal information to estimate audio track-relatedness. By applying Latent Semantic Indexing they embed corresponding textual information into a latent vector space from which they derive track relatedness for online triplet selection. This topic modelling facilitates fine-grained selection of similar and dissimilar audio-track pairs to learn the audio representation.  They show that the proposal is invariant to the variety of annotation styles as well as to the different languages of the collection. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabriella Pasi  is Full Professor at the Universit√† Degli Studi di Milano Bicocca. Within the Department of Informatics, Systems and Communication she is the head of the Information Retrieval Research Lab. Her research activity mainly concerns the modelling and design of flexible and personalised systems for the management and access to information (such as Information Retrieval Systems, and Information Filtering Systems), as well as the definition of  approaches to data analytics on social media. 
+She has published more than 200 papers on International Journals and Books, and on the Proceeding of International Conferences.  Since 2013 she is the President of the European Society for Fuzzy Logic and Technologies (EUSFLAT). She has delivered several Keynote Talks/Plenary Lectures at international conferences related to her research interests. She has participated to the organization of several International events, in both roles of organization and program chair.
+She is a member of the Editorial Board of several international journals among which the International Journal of Data Science and Analytics, Fuzzy Sets and Systems, the Journal of Computational Intelligence Systems, Intelligent Decision Technology: An International Journal.  She led several projects and she has been the coordinator of the European Project PENG (Personalized News Content Programming), a STREP (Specific Targeted Research or Innovation Project), within the VI Framework Programme, Priority II, Information Society Technology. Recently, she has been Member of the Management Committee (MC Member) of the COST ACTION IC1002: Multilingual and multifaceted interactive information access (MUMIA) (31/11/2010 ‚Äì 29/11/2014). Since 2002 she has co-organized the Information Access and Retrieval Track within the ACM SAC.
+Gloria Bordogna holds the position of senior researcher at the National Research Council Institute of Electromagnetic Sensing of the Environment CNR-IREA. In 2017 she was awarded fellow of the International Fuzzy System Association. From 2007 to 2010 she has been teaching Information Retrieval and Geographic Information Systems at the faculty of Engineering of Bergamo University. In 2011 she qualified for the position of director of research within CNR for the information systems scientific area. In 2013 she obtained the Italian National Scientific Qualification of full professor for the information systems scientific area. Her research activity concerns soft computing for managing imprecision and uncertainty affecting both textual and geographic information. She has defined adaptive indexing mechanisms and soft retrieval models for texts, images and geographic information, and flexible query languages to databases, to geographic information systems and social networks. She edited several volumes published by Springer Verlag, special issues of journals, and published over 200 papers in International Journals, in the proceedings of International Conferences and chapters in books. She is scientific responsible of several research projects,  program committee member of international Conferences such as ECIR, ACM CIKM, FQAS, FUZZIEEE, and serves as a reviewer of the European Science Foundation and journals such as JASIST, IEEE Trans. on Fuzzy Systems, Fuzzy Sets and Systems, IJGIS, IJGI .
+</t>
+  </si>
+  <si>
+    <t>2020/03/23 4:24:24 AM EST</t>
+  </si>
+  <si>
+    <t>francesco.santini@unipg.it</t>
+  </si>
+  <si>
+    <t>Knowledge Representation and Reasoning</t>
+  </si>
+  <si>
+    <t>KRR</t>
+  </si>
+  <si>
+    <t>http://www.dmi.unipg.it/bista/organizing/KRR@sac2020/</t>
+  </si>
+  <si>
+    <t>Francesco Santini, Dipartimento di Matematica e Informatica, University of Perugia, Italy</t>
+  </si>
+  <si>
+    <t>Stefano Bistarelli, Dipartimento di Matematica e Informatica, University of Perugia, Italy
+Martine Ceberio, Computer Science Department, University of Texas at El Paso, USA 
+Eric Monfroy, Informatique - Laboratoire LERIA, Universit√© d'Angers, France
+Francesco Santini, Dipartimento di Matematica e Informatica, University of Perugia, Italy</t>
+  </si>
+  <si>
+    <t>0000-0002-3935-4696</t>
+  </si>
+  <si>
+    <t>http://www.dmi.unipg.it/francesco.santini/images/picture2.jpg</t>
+  </si>
+  <si>
+    <t>2020/03/23 9:25:12 AM EST</t>
+  </si>
+  <si>
+    <t>donatello.conte@univ-tours.fr</t>
+  </si>
+  <si>
+    <t>Video Processing for Human Behavioral Analysis</t>
+  </si>
+  <si>
+    <t>VP-HBA</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/view/vp-hba-sac-2020</t>
+  </si>
+  <si>
+    <t>Donatello Conte, University of Tours, Computer Science Laboratory (LIFAT - EA 6300)</t>
+  </si>
+  <si>
+    <t>Donatello Conte - University of Tours, Computer Science Laboratory (LIFAT - EA 6300), chair
+Jean-Yves Ramel - University of Tours, Computer Science Laboratory (LIFAT - EA 6300), co-chair
+Raffaella Lanzarotti - University of Milano, Phuse Lab, co-chair</t>
+  </si>
+  <si>
+    <t>This track aimed to focus on all aspects of computer vision and pattern recognition devoted to the automatic analysis of human behavior by applying recent or new video processing techniques. Accepted papers mainly cover the following topics: Physiological Signal Estimation, Activities and Actions Recognition, Tracking, Gait Analysis and Emotion Analysis.
+We would like to thank all the Program Committee members for their help in the review process. We wish to thank all the local organizers that rearrange this conference in online mode. Finally, we want to thank all the contributors to this track for theirs valuable works.</t>
+  </si>
+  <si>
+    <t>0000-0003-4642-4768</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/donatello-conte-4210156/</t>
+  </si>
+  <si>
+    <t>https://scholar.google.fr/citations?user=dAKCYJgAAAAJ&amp;hl=fr</t>
+  </si>
+  <si>
+    <t>Donatello Conte received his Ph.D. degree in 2006 by a joint supervision between LIRIS laboratory of the INSA of Lyon (France) and MIVIA laboratory of the University of Salerno (Italy). 
+He has been an Assistant Professor from 2006 to 2013, in Italy at the University of Salerno. From 2013 to date, he is Associate Professor at the Computer Science Laboratory of the University of Tours. 
+His main research fields are: structural pattern recognition (graph matching, graph kernels, combinatorial maps), video analysis (objects detection and tracking, trajectories analysis, crowding estimation, etc.), and affective computing (emotion recognition, multimodality analysis for affective analysis, modeling affection, etc.). 
+He is the author of more than 70 publications and reviewers in the main journals in his research field (PAMI, PR, CVIU, TIP, etc.). He is member of the Editorial Board of the Elsevier Journal Internet of Things. He is currently Guest Editor for a Special Issue on graphs in pattern recognition in Elsevier Journal Pattern Recognition Letters.
+He is a member of the IAPR TC15 (dedicated to the promotion of graphs in the Pattern Recognition), for which he animates, with J.Y. Ramel, the TC15 Newsletter. He has been co-chair of the International Workshop on Graph-basd Representation in Pattern Recognition (GbR) held in Tours, France in June 2019. He is co-chair of the ACM/SAC Track on Video Processing for Human Behavioral Analysis.</t>
+  </si>
+  <si>
+    <t>2020/03/23 4:55:09 PM EST</t>
+  </si>
+  <si>
+    <t>cyril.derunz@univ-tours.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Geographical Information Analytics </t>
+  </si>
+  <si>
+    <t>GIA</t>
+  </si>
+  <si>
+    <t>https://gia.sciencesconf.org/</t>
+  </si>
+  <si>
+    <t>Cyril de Runz, BDTLN, LIFAT, University of Tours</t>
+  </si>
+  <si>
+    <t>Cyril de Runz, University of Tours, chair
+Eric Kergosien, University of Lille, chair
+Christian Sallaberry, University of Pau and Pays de l'Adour, chair
+Gavin McArdle, University College Dublin, chair</t>
+  </si>
+  <si>
+    <t>0000-0002-5951-6859</t>
+  </si>
+  <si>
+    <t>2020/03/24 12:40:50 AM EST</t>
+  </si>
+  <si>
+    <t>wook@hanyang.ac.kr</t>
+  </si>
+  <si>
+    <t>Social Network and Media Analysis</t>
+  </si>
+  <si>
+    <t>SONAMA</t>
+  </si>
+  <si>
+    <t>http://www.agape.hanyang.ac.kr/sonama2020</t>
+  </si>
+  <si>
+    <t>Sang-Wook Kim, Hanyang University, Korea</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=ed2vz_oAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>2020/03/24 8:42:14 AM EST</t>
+  </si>
+  <si>
+    <t>giamp@dmi.unict.it</t>
+  </si>
+  <si>
+    <t>Computer Security</t>
+  </si>
+  <si>
+    <t>SEC</t>
+  </si>
+  <si>
+    <t>http://www.dmi.unict.it/~giamp/sac/</t>
+  </si>
+  <si>
+    <t>Giampaolo Bella, University of Catania</t>
+  </si>
+  <si>
+    <t>Giampaolo Bella, University of Catania
+Rosario Giustolisi, IT University of Copenhagen</t>
+  </si>
+  <si>
+    <t>0000-0002-7615-8643</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/giampaolo-bella-a905315a/</t>
+  </si>
+  <si>
+    <t>https://scholar.google.it/citations?user=yBoGdJUAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>http://www.dmi.unict.it/~giamp/</t>
+  </si>
+  <si>
+    <t>2020/03/24 11:40:15 AM EST</t>
+  </si>
+  <si>
+    <t>rprocha@isr.uc.pt</t>
+  </si>
+  <si>
+    <t>Intelligent Robotics and Multi-Agent Systems</t>
+  </si>
+  <si>
+    <t>IRMAS</t>
+  </si>
+  <si>
+    <t>https://sac2020-irmas.isr.uc.pt</t>
+  </si>
+  <si>
+    <t>Rui P. Rocha, ISR - University of Coimbra, Portugal</t>
+  </si>
+  <si>
+    <t>Rui P. Rocha, ISR - University of Coimbra, Portugal, Chair
+Daniel Kudenko, L3S Research Center, Germany, Co-Chair
+Denis F. Wolf, ICMC - University of Sao Paulo, Brazil, Co-Chair</t>
+  </si>
+  <si>
+    <t>Many people have contributed to the success of this track. First of all, we would like to thank to all members of the international Program Committee (PC) for their efforts in attracting quality papers and in providing thoughtful reviews on time. We also want to thank all the authors who contributed to the SAC 2020 IRMAS track. Finally, we offer special thanks to the SAC 2020 Organizing Committee and the ACM SIGAPP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The special track on Intelligent Robotics and Multi-Agent Systems (IRMAS) focuses on all aspects of intelligent robotics and multi-agent systems (MAS) including related areas and applications. Its primary goal is to exploit synergies between robotics and artificial intelligence (AI), more precisely between intelligent robotics and MAS, and bring together researchers from both fields. For many years, robotics and AI researchers have worked separately, both fields have matured enormously, and today there is a growing interest in getting the two research fields together. Many in robotics believe that the focus in the near future should be adding capabilities to robots that lie at the core of AI research. Reciprocally, AI researchers aim at embedding their techniques in physical robots that can perceive, reason and act in real, dynamic environments.
+In this sixth edition, there were 23 papers submitted from Europe (10), South America (4), North America (2), South Asia (2), North Africa (2), Middle East (2), and Far East (1). After a rigorous blind peer review process by 65 PC members, 6 regular papers and 3 poster papers were accepted to be presented in the SAC 2020 IRMAS track. The accepted papers cover important topics of this track, both on intelligent robotics and MAS, namely multi-robot path planning, multi-robot coalition formation, cooperative transportation, robot trajectory generation, social robot navigation, distributed planning under uncertainty, multi-agent routing, and agent-oriented design of cyber-physical systems.
+</t>
+  </si>
+  <si>
+    <t>0000-0002-4612-3554</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=L4dw8sIAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>Rui P. Rocha is an assistant professor in the Dept. of Electrical and Computer Engineering and a senior researcher of the Institute of Systems and Robotics at the University of Coimbra, Portugal. His main research interests are multi-robot systems, cooperative perception, distributed control, autonomous robots, and ambient assisted living. He was one of the founders of the IRMAS track and was co-chair of all 6 editions.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1NiT2-ObnMYLzVXP6qBp-wN-R5sZLd4Tr/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>2020/03/25 8:36:53 AM EST</t>
+  </si>
+  <si>
+    <t>lpchang@cs.nctu.edu.tw</t>
+  </si>
+  <si>
+    <t>Embedded Systems</t>
+  </si>
+  <si>
+    <t>EMBS</t>
+  </si>
+  <si>
+    <t>https://sac2020.cs.nctu.edu.tw/</t>
+  </si>
+  <si>
+    <t>Marco Di Natale, Scuola Superiore S. Anna, Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the Embedded Systems track! This year is the 20th edition of this highly successful track in the SAC series. The track program covers non-volatile memory, automotive systems, MPSoCs, real-time systems, and system tools (not an exhaustive listing). We track co-chairs hope that all the virtual attendees enjoy our rich program. </t>
+  </si>
+  <si>
+    <t>0000-0001-6543-2064</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=t21ZkxEAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>Li-Pin Chang received the M.S.E. and Ph.D. degrees in computer science and information engineering from National Taiwan University, Taipei, Taiwan, in 1997 and 2003, respectively. He is currently a Professor with the Department of Computer Science, College of Computer Science, National Chiao Tung University, Hsinchu, Taiwan, ROC. His current research interests include operating systems, storage systems, non-volatile memory, and mobile devices.</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/view/lpchang</t>
+  </si>
+  <si>
+    <t>2020/03/25 1:50:44 PM EST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geographical Information Analytics </t>
+  </si>
+  <si>
+    <t>Christian Sallaberry, University of PAU &amp; PAYS ADOUR, LIUPPA lab., France, chair
+Eric Kergosien, University of LILLE, GERiiCO lab, France, chair
+Cyril de Runz, BDTLN/LIFAT University of Tours, France, chair
+Gavin Mcardle, UCD School of Computer Science, University College Dublin, chair
+Luis Otavio Alvares, Universidade Federal de Santa Catarina, chair</t>
+  </si>
+  <si>
+    <t>Unfortunately, the face-to-face meeting has been cancelled and converted to an online format where authors are required to submit their video presentation on the website.
+Dear authors, please don‚Äôt forget to provide your online presentation.
+If you face any problem, please contact us or Dr. Junyoung Heo, the registrar of the conference, at jyheo@hansung.ac.kr</t>
+  </si>
+  <si>
+    <t>2020/03/26 2:50:36 AM EST</t>
+  </si>
+  <si>
+    <t>matthias@guedemann.org</t>
+  </si>
+  <si>
+    <t>Software Verification and Testing Track</t>
+  </si>
+  <si>
+    <t>SVT</t>
+  </si>
+  <si>
+    <t>https://guedemann.org/svt2020/</t>
+  </si>
+  <si>
+    <t>matthias.guedemann@hm.edu</t>
+  </si>
+  <si>
+    <t>Nikolai Kosmatov, CEA List &amp; Thales, chair
+Matthias G√ºdemann, University of Applied Sciences Munich, chair</t>
+  </si>
+  <si>
+    <t>Welcome to the Software Verification and Testing track of SAC 2020!
+The Software Verification and Testing (SVT) track of SAC aims at contributing to the challenge of improving the usability of program verification and validation techniques in software engineering. The track covers various areas of formal methods and testing. The authors are invited to submit new results, as well as technologies to improve their usability in software engineering. The track also welcomes surveys, descriptions of benchmarks and applications to large-scale software.
+SVT has been a part of SAC since 2010, and since then has been a forum for interesting presentations and fruitful discussions. This year, the SVT track received 37 submissions. All papers went through a rigorous reviewing process, where each paper was reviewed by three members of the track Program Committee. The selection process was very competitive. After an active discussion, 10 papers were selected for acceptance and the final versions for 9 papers were finally submitted for publication. They cover a large range of topics of formal verification and testing. We thank the Program Committee members for their hard work during the paper selection process.
+Due to the COVID-19 pandemic, the face-to-face meeting was not possible this year and was replaced by an online conference. We hope that the Software Verification and Testing (SVT) track of SAC 2020 will still offer to SAC participants a rich and challenging program.
+The SVT track co-chairs,
+Matthias G√ºdemann and Nikolai Kosmatov</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-1557-2813</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/nikolay-kosmatov-69a22862/</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=ieueHysAAAAJ&amp;hl=en&amp;oi=ao</t>
+  </si>
+  <si>
+    <t>2020/03/26 7:09:59 AM EST</t>
+  </si>
+  <si>
+    <t>esposito@unisa.it</t>
+  </si>
+  <si>
+    <t>Sustainability of Fog/Edge Computing Systems Track</t>
+  </si>
+  <si>
+    <t>SFECS</t>
+  </si>
+  <si>
+    <t>https://sfecs.di.unisa.it/</t>
+  </si>
+  <si>
+    <t>Florin Pop, University Politehnica of Bucharest, Romania, Chang Choi, Chosun University, Rep. of Korea, Xin Su, Hohai University, China</t>
+  </si>
+  <si>
+    <t>0000-0002-0085-0748</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/christianesposito/</t>
+  </si>
+  <si>
+    <t>https://scholar.google.it/citations?user=mA0OypkAAAAJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gloria Bordogna, CNR IREA </t>
+  </si>
+  <si>
+    <t>Li-Pin Chang, National Chiao Tung University</t>
+  </si>
+  <si>
+    <t>Cyril de Runz, BDTLN/LIFAT University of Tours, France, chair</t>
+  </si>
+  <si>
+    <t>Matthias Guedemann, University of Applied Sciences Munich</t>
+  </si>
+  <si>
+    <t>Christian Esposito, University of Salerno, Italy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1006,12 +1426,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="99" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1104,7 +1532,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1136,7 +1564,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1166,6 +1594,491 @@
       </c>
       <c r="L4" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
+      </c>
+      <c r="M6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M9" t="s">
+        <v>87</v>
+      </c>
+      <c r="N9" t="s">
+        <v>88</v>
+      </c>
+      <c r="O9" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" t="s">
+        <v>100</v>
+      </c>
+      <c r="O11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M12" t="s">
+        <v>113</v>
+      </c>
+      <c r="N12" t="s">
+        <v>114</v>
+      </c>
+      <c r="O12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G13" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J13" t="s">
+        <v>124</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M13" t="s">
+        <v>126</v>
+      </c>
+      <c r="O13" t="s">
+        <v>127</v>
+      </c>
+      <c r="P13" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" t="s">
+        <v>166</v>
+      </c>
+      <c r="H14" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" t="s">
+        <v>135</v>
+      </c>
+      <c r="L14" t="s">
+        <v>136</v>
+      </c>
+      <c r="M14" t="s">
+        <v>137</v>
+      </c>
+      <c r="O14" t="s">
+        <v>138</v>
+      </c>
+      <c r="P14" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" t="s">
+        <v>167</v>
+      </c>
+      <c r="H15" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>149</v>
+      </c>
+      <c r="G16" t="s">
+        <v>168</v>
+      </c>
+      <c r="H16" t="s">
+        <v>150</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M16" t="s">
+        <v>153</v>
+      </c>
+      <c r="N16" t="s">
+        <v>154</v>
+      </c>
+      <c r="O16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G17" t="s">
+        <v>169</v>
+      </c>
+      <c r="H17" t="s">
+        <v>157</v>
+      </c>
+      <c r="I17" t="s">
+        <v>161</v>
+      </c>
+      <c r="M17" t="s">
+        <v>162</v>
+      </c>
+      <c r="N17" t="s">
+        <v>163</v>
+      </c>
+      <c r="O17" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added slides url postprocessing, fixed imports
</commit_message>
<xml_diff>
--- a/app-server/src/main/resources/chairs_responses.xlsx
+++ b/app-server/src/main/resources/chairs_responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/code/acmsac/app-server/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF85867-C2BC-AF43-99DF-59CFB6A5870B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD77C4D-8B79-1E40-B3EA-CB4A0CC9323B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="940" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chairs_test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="195">
   <si>
     <t>Timestamp</t>
   </si>
@@ -585,12 +585,115 @@
   <si>
     <t>Christian Esposito, University of Salerno, Italy</t>
   </si>
+  <si>
+    <t>2020/03/27 1:36:49 PM EST</t>
+  </si>
+  <si>
+    <t>matteo.camilli@unibz.it</t>
+  </si>
+  <si>
+    <t>Software Architecture: Theory, Technology, and Applications</t>
+  </si>
+  <si>
+    <t>SA-TTA</t>
+  </si>
+  <si>
+    <t>https://dinamico2.unibg.it/sa-tta/2020/</t>
+  </si>
+  <si>
+    <t>Matteo Camilli, Free University of Bozen-Bolzano, Italy</t>
+  </si>
+  <si>
+    <t>mtteo.camilli@unibz.it</t>
+  </si>
+  <si>
+    <t>Matteo Camilli, Free University of Bozen-Bolzano, Italy
+Patrizia Scandurra, University of Bergamo, Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software Architecture is a consolidated and necessary discipline centered on the idea of reducing complexity in software development and evolution through abstraction and separation of concerns. The goal of the track SA-TTA is to bring together researchers, practitioners and educators having the common objective of transforming Software Architecture into a mature discipline leveraging on both solid scientific foundations and validated engineering methodologies and tools.  The main focus is in Applied Software Architecture, namely practical engineering concerns, experiences in tools development, and software architecture case studies. SA-TTA is focused broadly on how to address functional requirements and quality characteristics in the design, maintenance, and adaptation and evolution of software architectures through the support of automated techniques and tools. Of special interest are architecture description languages, formalisms, techniques, methodologies, tools, and runtime environments that support these activities, possibly exploiting model-driven engineering principles. A special emphasis is put also on technical aspects of software architectures development for specific class of software systems and application domains.
+This year the track received interdisciplinary research contributions covering a variety of topics related to: architectural styles for Internet of Things and Cloud of Things platforms, trustability and security concerns in Blockchain based choreographies, model-based development of microservice architectures, and domain engineering.
+The track co-chairs would like to thank all the authors for their valuable contribution and their lat-minute effort to deal with the current difficult situation. All the organizers made their best to give SAC participants the opportunity to share their research results, and possibly discuss any related aspects without threatening the health and safety of persons.
+We hope that participants can find meaningful sources of information through the SAC online platform. 
+Sincerely,
+Matteo and Patrizia
+SA-TTA track co-chairs </t>
+  </si>
+  <si>
+    <t>0000-0003-2491-5267</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=zFC7S-8AAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>Matteo Camilli:
+Matteo is currently an assistant professor at the Faculty of Computer Science of the Free University of Bozen-Bolzano (Italy). His recent teaching activities include M.Sc. courses on software and systems engineering, formal methods, and verification of dependable systems. He is part of the software and systems engineering research group headed by prof. Barbara Russo. Matteo received the PhD degree in Computer Science from the University of Milan in 2014. His dissertation focused on the combination of advanced abstraction techniques and big data approaches to tackle the state explosion problem in formal verification. His current research activity focuses on Formal Methods and Software Engineering. He is especially interested in: software requirements specification, analysis and verification; Model-based testing; Uncertainty quantification along the software lifecycle; runtime verification methods; formal modeling using Markov models; models of concurrency such as Petri Nets; and the application of methodologies, theories, approaches and techniques specific to the above research areas to complex, advanced, distributed, time-dependent, service-oriented, component-based and self-adaptive systems. He publishes papers in international journals and in proceedings of international conferences. He serves as member of the program committee of international conferences.
+Patrizia Scandurra:
+Patrizia Scandurra is Associate Professor at the Department of Information Technologies(DTI) of the University of Milan (Italy). From January 2009 till October 2018 she was assistant professor at the Department of Management, Information and Production Engineering of the University of Bergamo (Italy). She teaches courses of software design/programming and operating systems. Her research field of interest is Software Engineering and, in particular, the areas of formal methods for the design and analysis of software systems, software architectures, and model-driven engineering. Her research interests include: definition and integration of theories, languages and techniques specific to the above research areas, and their application to distributed self-adaptive software systems, service-oriented and cloud-based systems, IoT applications, embedded systems and systems-on-chip. She has published over 80 research articles in international journals and conferences. She is an active member of the Abstract State Machines (ASM) formal method community. She regularly serves in international program committees and as a referee for top-ranked journals. She has been involved in national and European projects on themes such as model-driven development for embedded and robotic systems, and adaptive software architectures for pervasive systems. She collaborated with Italian R&amp;I (research and innovation) groups of industries like STMicroelectronics and Atego and with the ENEA Smart Cities &amp; Communities lab.</t>
+  </si>
+  <si>
+    <t>https://matteocamilli.github.io/authors/admin/avatar_huf9975595e9221e8c10f56e790d7e497e_843959_250x250_fill_lanczos_center_2.png</t>
+  </si>
+  <si>
+    <t>2020/03/28 7:27:46 AM EST</t>
+  </si>
+  <si>
+    <t>priya@nitc.ac.in</t>
+  </si>
+  <si>
+    <t>Cloud Computing</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/nitc.ac.in/acmsac2020-cloudcomputingtrack/home</t>
+  </si>
+  <si>
+    <t>Madhu Kumar S D,  National Institute  of Technology Calicut, Chair
+Priya Chandran,  National Institute  of Technology Calicut, Chair</t>
+  </si>
+  <si>
+    <t>Track Program Committee, Authors, NIT Calicut, ACM, SIGAPP</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=V-DXftkAAAAJ&amp;hl=en&amp;oi=ao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Dr.S.D Madhu Kumar is a Professor in the Department of Computer Science &amp;amp; Engineering
+of National Institute of Technology Calicut. For the past 27 years he has been working in the
+Computer Science &amp;amp; Engineering Department of National Institute of Technology Calicut
+(NIT Calicut), which is a centrally funded institute of National Importance in India. He was
+the Head of the Computer Science &amp;amp; Engineering dept of NIT Calicut during 2012-2014.
+Currently he is the Dean( Students‚Äô Welfare) of NIT Calicut. Dr. S.D Madhu Kumar received
+his PhD in Computer Science &amp;amp; Engineering from the Indian Institute of Technology Bombay
+(IIT Bombay). Earlier he did his Masters in Engineering in Computer Science &amp;amp; Engineering
+from Indian Institute of Science, Bangalore ( IISc Bangalore), India. He has more than 60
+International publications to his credit and has produced seven PhDs and currently guiding six
+Doctoral students at NIT Calicut. His research interests include Cloud Computing, Big Data
+Analytics, Software Engineering and DBMS. He is a senior member of IEEE and a member
+of ACM USA. He has been the chair and keynote speaker for many International
+Conferences. He has been the Track Co-chair of the Cloud Computing Track of the ACM
+Symposium on Applied Computing ( SAC) since 2010. He also serves in the editorial board
+of several international journals including ACM ACR.
+More details of Dr. Madhu can be found at http://people.cse.nitc.ac.in/madhu</t>
+  </si>
+  <si>
+    <t>http://people.cse.nitc.ac.in/madhu/</t>
+  </si>
+  <si>
+    <t>Priya Chandran, National Institute of Technology Calicut</t>
+  </si>
+  <si>
+    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/gdHY2UIT4C8" frameborder="0" allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -725,6 +828,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1023,7 +1134,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1066,14 +1177,16 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1107,6 +1220,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1427,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1439,6 +1553,7 @@
     <col min="7" max="7" width="99" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="77.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -1596,7 +1711,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" ht="221" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1733,7 +1848,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -1777,7 +1892,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" ht="306" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -1838,7 +1953,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="136" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>106</v>
       </c>
@@ -1879,7 +1994,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>117</v>
       </c>
@@ -2043,7 +2158,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>156</v>
       </c>
@@ -2079,6 +2194,94 @@
       </c>
       <c r="O17" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" t="s">
+        <v>176</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M18" t="s">
+        <v>179</v>
+      </c>
+      <c r="O18" t="s">
+        <v>180</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>187</v>
+      </c>
+      <c r="G19" t="s">
+        <v>193</v>
+      </c>
+      <c r="H19" t="s">
+        <v>184</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J19" t="s">
+        <v>189</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="O19" t="s">
+        <v>190</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed another URL overflow; data update
</commit_message>
<xml_diff>
--- a/app-server/src/main/resources/chairs_responses.xlsx
+++ b/app-server/src/main/resources/chairs_responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/code/acmsac/app-server/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F3B75D-4B08-6341-8FE1-4B2935EB203C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2C6E3E-A20A-7948-9D78-1C20ABF08AC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="940" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="1600" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chairs_test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="312">
   <si>
     <t>Timestamp</t>
   </si>
@@ -801,6 +801,268 @@
   </si>
   <si>
     <t>Maria Lencastre, Universidade de Pernambuco</t>
+  </si>
+  <si>
+    <t>2020/03/29 7:20:37 PM EST</t>
+  </si>
+  <si>
+    <t>cristian.mateos@isistan.unicen.edu.ar</t>
+  </si>
+  <si>
+    <t>Web Technologies</t>
+  </si>
+  <si>
+    <t>WT</t>
+  </si>
+  <si>
+    <t>http://www.cs.unibo.it/projects/sacwt20/</t>
+  </si>
+  <si>
+    <t>Tim A. Majchrzak, University of Agder - Kristiansand, Norway
+Francesco Poggi, University of Bologna - Bologna, Italy</t>
+  </si>
+  <si>
+    <t>We thank the reviewers for their support in reviewing the papers submitted to the track.</t>
+  </si>
+  <si>
+    <t>0000-0001-5761-1898</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=DAf6BckAAAAJ&amp;hl=es&amp;oi=ao</t>
+  </si>
+  <si>
+    <t>Cristian Mateos received a PhD degree in Computer Science from the
+UNICEN University in 2008. He is a full-time Adjunct Professor at
+the UNICEN and member of ISISTAN-CONICET. His main research interest
+are parallel/distributed programming, Grid/Cloud middlewares and Service-
+oriented Computing.</t>
+  </si>
+  <si>
+    <t>http://users.exa.unicen.edu.ar/~cmateos/images/image.jpg</t>
+  </si>
+  <si>
+    <t>2020/03/29 9:42:56 PM EST</t>
+  </si>
+  <si>
+    <t>Barrett.Bryant@unt.edu</t>
+  </si>
+  <si>
+    <t>Programming Languages</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>http://www.cse.unt.edu/~bryant/sac2020/</t>
+  </si>
+  <si>
+    <t>Barrett Bryant, University of North Texas, Co-Chair
+Rajeev Raje, Indiana University Purdue University Indianapolis, Co-Chair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We would like to thank all authors for their valuable contributions. We also thank the program committee members who voluntarily supported us to recruit good papers and review the papers. </t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-9505-5351?lang=en</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/barrett-bryant-a0310b1/</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=hMCK39sAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>Barrett R. Bryant is Professor and Chair of Computer Science and Engineering (CSE) at the University of North Texas (UNT). He received his B. S. in computer science from the University of Arkansas at Little Rock in 1979 and his M. S. and Ph. D. in computer science from Northwestern University in 1980 and 1983, respectively. From 1983-2011, he was on the faculty of the University of Alabama at Birmingham. He has also held visiting appointments at a number of institutions, including Ibaraki University, Hitachi, Japan, the Naval Postgraduate School, Monterey, California, USA, and Tsinghua University, Beijing, China. He serves on the Steering Committee of SAC (ACM Symposium on Applied Computing), and is a member of EAPLS, and a senior member of ACM and IEEE. His primary research area is programming languages, especially applied to problems in software engineering, and has published over 150 papers in journals and conferences in this and related fields. Further details are available at http://www.cse.unt.edu/~bryant.</t>
+  </si>
+  <si>
+    <t>http://www.cse.unt.edu/~bryant</t>
+  </si>
+  <si>
+    <t>2020/03/30 1:42:19 AM EST</t>
+  </si>
+  <si>
+    <t>klp@fbk.eu</t>
+  </si>
+  <si>
+    <t>Knowledge and Language Processing</t>
+  </si>
+  <si>
+    <t>KLP</t>
+  </si>
+  <si>
+    <t>https://klp.fbk.eu/</t>
+  </si>
+  <si>
+    <t>Marco Rospocher, University of Verona</t>
+  </si>
+  <si>
+    <t>marco.rospocher@univr.it</t>
+  </si>
+  <si>
+    <t>Mauro Dragoni, FBK, co-chair</t>
+  </si>
+  <si>
+    <t>Aim of the Knowledge and Language Processing (KLP) track at ACM SAC is to investigate techniques and application of knowledge engineering and natural language processing, focusing in particular on approaches combining them. This is an extremely interdisciplinary emerging research area, at the core of Artificial Intelligence, combining and complementing the scientific results from Natural Language Processing and Knowledge Representation and Reasoning.</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=wkAcWjMAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>https://scholar.googleusercontent.com/citations?view_op=medium_photo&amp;user=wkAcWjMAAAAJ&amp;citpid=6</t>
+  </si>
+  <si>
+    <t>2020/03/30 4:30:08 AM EST</t>
+  </si>
+  <si>
+    <t>mzanker@unibz.it</t>
+  </si>
+  <si>
+    <t>Recommender Systems: Theory, User Interactions &amp; Applications</t>
+  </si>
+  <si>
+    <t>RecSys</t>
+  </si>
+  <si>
+    <t>https://recsystrack.wordpress.com/</t>
+  </si>
+  <si>
+    <t>Markus Zanker, Free University of Bozen-Bolzano</t>
+  </si>
+  <si>
+    <t>Markus Zanker, Free University of Bozen-Bolzano, Panagiotis Symeonidis, Free University of Bozen-Bolzano, Yong Zheng, Illinois Institute of Technology</t>
+  </si>
+  <si>
+    <t>The organizers would like to particularly acknowledge the support and contribution by the expert program committee who provided valuable reviews.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the 6th issue of a track on RecSys research associated with ACM SAC! We received 23 valid submissions and after a rigorous review process 4 long papers and 2 short papers were selected for this track. Despite of current circumstances we hope these works will nevertheless receive readership and appreciation. Best wishes, the track co-chairs </t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-4805-5516</t>
+  </si>
+  <si>
+    <t>https://it.linkedin.com/in/markuszanker</t>
+  </si>
+  <si>
+    <t>https://scholar.google.at/citations?user=byE_7C8AAAAJ&amp;hl=de</t>
+  </si>
+  <si>
+    <t>https://campus.aau.at/vk/visitenkartenimage/image/245263613</t>
+  </si>
+  <si>
+    <t>2020/03/30 10:09:56 AM EST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We would like to thank all authors for really great submissions. In addition, we like to acknowledge all the track committees.
+PLEASE NOTE: We just received an email from Hindawi who reopens our special issue till July 3rd. https://www.hindawi.com/journals/sp/si/716070/ Please contact us in case you are submitting an extended version of your article. </t>
+  </si>
+  <si>
+    <t>2020/03/30 2:42:12 PM EST</t>
+  </si>
+  <si>
+    <t>anu.chacko@nitc.ac.in</t>
+  </si>
+  <si>
+    <t>Health Informatics</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?client=safari&amp;rls=en&amp;q=health+informatics+acm+sac+2020&amp;ie=UTF-8&amp;oe=UTF-8</t>
+  </si>
+  <si>
+    <t>Dr. Anu Mary Chacko, National Institute of Technology, Calicut, India</t>
+  </si>
+  <si>
+    <t>Gopakumar G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/4bQ1YHpbZGY" frameborder="0" allow="accelerometer; autoplay; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hi I am Anu Chacko. I teach in the National Institute of Technology of Calicut, India. I along with my colleague Gopa Kumar G has worked as track chairs for Health Informatics track in ACM SAC 2020.
+Health Informatics is an upcoming research field and is receiving a lot of attention from researchers all over the world as it works on ultimately improving human life by providing ideas for better proactive health care. Today as the hospitals are using Electronic Health Records, there is a large amount of data that is available. This data has its own privacy and security concerns. Much of the data is unstructured and there are large mines of information that needs to be discovered. Thus ACM SAC 2020 is the very apt place for discussing this field converging medicine and information technology. 
+This year we received around 19 papers in this track out of which 6 was accepted as paper and 1 as poster.  Papers looked at range of problem from extracting and undesrstanding semantic  information from HER to use of image processing, machine learning, IoT and agent based approaches for different medical problems. 
+Though we do not have a face to face engagement I hope that through this web platform we will be able to engage actively so as to further research in Health Informatics. 
+Thanks again 
+</t>
+  </si>
+  <si>
+    <t>http://people.cse.nitc.ac.in/achacko/</t>
+  </si>
+  <si>
+    <t>2020/03/30 2:42:51 PM EST</t>
+  </si>
+  <si>
+    <t>amm@fct.unl.pt</t>
+  </si>
+  <si>
+    <t>Ana Moreira</t>
+  </si>
+  <si>
+    <t>Ana Moreira, Universidade Nova de Lisboa</t>
+  </si>
+  <si>
+    <t>Ana Moreira, Universidade Nova de Lisboa, chair, Julio Cesar Leite, PUC-Rio, chair, Maria Lencastre, UPE, chair</t>
+  </si>
+  <si>
+    <t>Thank you to the organisers for coping with the difficulties we face today and making the conference still possible.</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Dn5txsRFHjU</t>
+  </si>
+  <si>
+    <t>0000-0003-2046-2766</t>
+  </si>
+  <si>
+    <t>https://scholar.google.com/citations?user=uB4MBw4AAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>Ana Moreira is an Associate Professor with Habilitation at Universidade Nova de Lisboa where she leads the Software Engineering group. Her main research topics are requirements engineering, architecture design, model-driven development, software quality, sustainability engineering, variability and trade-off analysis. She is or was a member of several editorial boards (TSE, SoSyM, TAOSD). She has been or still is a member of the Steering Committee for UML/MODELS, RE, AOSD/Modularity and PC member of numerous international conferences (e.g., MODELS, RE, ICSE, CAiSE). She has co-organized various international workshops and is co-founder of the international movements pUML and Early Aspects. She is or was Conference Chair and PC Chair of several international events, such co-General Chair for RE 2017, and PC co-chair for AOSD‚Äô09, Foundations Track Chair for MODELS 2013, ACM SAC-RE‚Äô20, ICT4S‚Äô20, ISD‚Äô20 Track Chair and RE‚Äô21.</t>
+  </si>
+  <si>
+    <t>http://ctp.di.fct.unl.pt/~amm/</t>
+  </si>
+  <si>
+    <t>2020/03/30 5:48:12 PM EST</t>
+  </si>
+  <si>
+    <t>mario@di.ubi.pt</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>NET</t>
+  </si>
+  <si>
+    <t>http://www.di.ubi.pt/sac2020/</t>
+  </si>
+  <si>
+    <t>Mario M. Freire, University of Beira Interior, Portugal</t>
+  </si>
+  <si>
+    <t>M√°rio M. Freire, University of Beira Interior, Co-Chair
+Mar√≠lia Curado, University of Coimbra, Co-Chair
+Ivan Ganchev, University of Limerick/University of Plovdiv ‚ÄúPaisii Hilendarski‚Äù, Co-Chair
+Mohamed Mosbah, LaBRI, Co-chair</t>
+  </si>
+  <si>
+    <t>http://orcid.org/0000-0002-9017-5001</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/mario-freire-222b237/</t>
+  </si>
+  <si>
+    <t>http://www.di.ubi.pt/~mario/</t>
+  </si>
+  <si>
+    <t>Cristian Mateos Diaz, ISISTAN-UNICEN-CONICET, Tandil, Argentina</t>
+  </si>
+  <si>
+    <t>Barrett R Bryant, University of North Texas</t>
   </si>
 </sst>
 </file>
@@ -1655,10 +1917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2533,6 +2795,361 @@
         <v>228</v>
       </c>
     </row>
+    <row r="23" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23" t="s">
+        <v>231</v>
+      </c>
+      <c r="C23" t="s">
+        <v>232</v>
+      </c>
+      <c r="D23" t="s">
+        <v>233</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>234</v>
+      </c>
+      <c r="G23" t="s">
+        <v>310</v>
+      </c>
+      <c r="H23" t="s">
+        <v>231</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J23" t="s">
+        <v>236</v>
+      </c>
+      <c r="M23" t="s">
+        <v>237</v>
+      </c>
+      <c r="O23" t="s">
+        <v>238</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="204" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>241</v>
+      </c>
+      <c r="B24" t="s">
+        <v>242</v>
+      </c>
+      <c r="C24" t="s">
+        <v>243</v>
+      </c>
+      <c r="D24" t="s">
+        <v>244</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>245</v>
+      </c>
+      <c r="G24" t="s">
+        <v>311</v>
+      </c>
+      <c r="H24" t="s">
+        <v>242</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J24" t="s">
+        <v>247</v>
+      </c>
+      <c r="M24" t="s">
+        <v>248</v>
+      </c>
+      <c r="N24" t="s">
+        <v>249</v>
+      </c>
+      <c r="O24" t="s">
+        <v>250</v>
+      </c>
+      <c r="P24" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" t="s">
+        <v>254</v>
+      </c>
+      <c r="C25" t="s">
+        <v>255</v>
+      </c>
+      <c r="D25" t="s">
+        <v>256</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>257</v>
+      </c>
+      <c r="G25" t="s">
+        <v>258</v>
+      </c>
+      <c r="H25" t="s">
+        <v>259</v>
+      </c>
+      <c r="I25" t="s">
+        <v>260</v>
+      </c>
+      <c r="L25" t="s">
+        <v>261</v>
+      </c>
+      <c r="O25" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>264</v>
+      </c>
+      <c r="B26" t="s">
+        <v>265</v>
+      </c>
+      <c r="C26" t="s">
+        <v>266</v>
+      </c>
+      <c r="D26" t="s">
+        <v>267</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>268</v>
+      </c>
+      <c r="G26" t="s">
+        <v>269</v>
+      </c>
+      <c r="H26" t="s">
+        <v>265</v>
+      </c>
+      <c r="I26" t="s">
+        <v>270</v>
+      </c>
+      <c r="J26" t="s">
+        <v>271</v>
+      </c>
+      <c r="L26" t="s">
+        <v>272</v>
+      </c>
+      <c r="M26" t="s">
+        <v>273</v>
+      </c>
+      <c r="N26" t="s">
+        <v>274</v>
+      </c>
+      <c r="O26" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B27" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" t="s">
+        <v>197</v>
+      </c>
+      <c r="D27" t="s">
+        <v>198</v>
+      </c>
+      <c r="E27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" t="s">
+        <v>199</v>
+      </c>
+      <c r="G27" t="s">
+        <v>200</v>
+      </c>
+      <c r="H27" t="s">
+        <v>196</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="K27" t="s">
+        <v>203</v>
+      </c>
+      <c r="L27" t="s">
+        <v>204</v>
+      </c>
+      <c r="M27" t="s">
+        <v>205</v>
+      </c>
+      <c r="N27" t="s">
+        <v>206</v>
+      </c>
+      <c r="O27" t="s">
+        <v>207</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>279</v>
+      </c>
+      <c r="B28" t="s">
+        <v>280</v>
+      </c>
+      <c r="C28" t="s">
+        <v>281</v>
+      </c>
+      <c r="D28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" t="s">
+        <v>283</v>
+      </c>
+      <c r="G28" t="s">
+        <v>284</v>
+      </c>
+      <c r="H28" t="s">
+        <v>280</v>
+      </c>
+      <c r="I28" t="s">
+        <v>285</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>289</v>
+      </c>
+      <c r="B29" t="s">
+        <v>290</v>
+      </c>
+      <c r="C29" t="s">
+        <v>291</v>
+      </c>
+      <c r="D29" t="s">
+        <v>213</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" t="s">
+        <v>214</v>
+      </c>
+      <c r="G29" t="s">
+        <v>292</v>
+      </c>
+      <c r="H29" t="s">
+        <v>290</v>
+      </c>
+      <c r="I29" t="s">
+        <v>293</v>
+      </c>
+      <c r="J29" t="s">
+        <v>294</v>
+      </c>
+      <c r="K29" t="s">
+        <v>295</v>
+      </c>
+      <c r="M29" t="s">
+        <v>296</v>
+      </c>
+      <c r="O29" t="s">
+        <v>297</v>
+      </c>
+      <c r="P29" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="372" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>300</v>
+      </c>
+      <c r="B30" t="s">
+        <v>301</v>
+      </c>
+      <c r="C30" t="s">
+        <v>302</v>
+      </c>
+      <c r="D30" t="s">
+        <v>303</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
+        <v>304</v>
+      </c>
+      <c r="G30" t="s">
+        <v>305</v>
+      </c>
+      <c r="H30" t="s">
+        <v>301</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="M30" t="s">
+        <v>307</v>
+      </c>
+      <c r="N30" t="s">
+        <v>308</v>
+      </c>
+      <c r="O30" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>309</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>